<commit_message>
plot_accuracy_vs_epoch.py can now make boxplots for groups of epochs
</commit_message>
<xml_diff>
--- a/Neurosim/data/128_src_is_500ltpltd.xlsx
+++ b/Neurosim/data/128_src_is_500ltpltd.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1259"/>
+  <dimension ref="A1:B1251"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10445,70 +10445,6 @@
         <v>87</v>
       </c>
     </row>
-    <row r="1252">
-      <c r="A1252" s="1" t="n">
-        <v>1251</v>
-      </c>
-      <c r="B1252" t="n">
-        <v>86.76000000000001</v>
-      </c>
-    </row>
-    <row r="1253">
-      <c r="A1253" s="1" t="n">
-        <v>1252</v>
-      </c>
-      <c r="B1253" t="n">
-        <v>89.48</v>
-      </c>
-    </row>
-    <row r="1254">
-      <c r="A1254" s="1" t="n">
-        <v>1253</v>
-      </c>
-      <c r="B1254" t="n">
-        <v>88.18000000000001</v>
-      </c>
-    </row>
-    <row r="1255">
-      <c r="A1255" s="1" t="n">
-        <v>1254</v>
-      </c>
-      <c r="B1255" t="n">
-        <v>89.84</v>
-      </c>
-    </row>
-    <row r="1256">
-      <c r="A1256" s="1" t="n">
-        <v>1255</v>
-      </c>
-      <c r="B1256" t="n">
-        <v>89.62</v>
-      </c>
-    </row>
-    <row r="1257">
-      <c r="A1257" s="1" t="n">
-        <v>1256</v>
-      </c>
-      <c r="B1257" t="n">
-        <v>90.14</v>
-      </c>
-    </row>
-    <row r="1258">
-      <c r="A1258" s="1" t="n">
-        <v>1257</v>
-      </c>
-      <c r="B1258" t="n">
-        <v>84.34999999999999</v>
-      </c>
-    </row>
-    <row r="1259">
-      <c r="A1259" s="1" t="n">
-        <v>1258</v>
-      </c>
-      <c r="B1259" t="n">
-        <v>88.15000000000001</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>